<commit_message>
fixed # of arg for write
</commit_message>
<xml_diff>
--- a/Assignment4/databaseSchema.xlsx
+++ b/Assignment4/databaseSchema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\Documents\SemJ2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\Documents\CPSC_courses\CPSC408\CPSC408Submissions\Assignment4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DAC218-4DE9-4C1D-9500-133C49C957F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB096B6-8599-4C08-AC4F-EFF91F7197DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,14 +359,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -381,7 +381,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5194300" y="2927350"/>
+          <a:off x="5194300" y="4629150"/>
           <a:ext cx="1143000" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -422,14 +422,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -444,7 +444,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="755650" y="2927350"/>
+          <a:off x="755650" y="4629150"/>
           <a:ext cx="1143000" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -833,6 +833,216 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>473075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB5B6E97-6663-4D66-9FB8-32B2AA8FA817}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2987675" y="4635500"/>
+          <a:ext cx="1143000" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Employee</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ToShelther</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EADE824-9EAD-41C5-8CC3-9603C388D7E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5194300" y="2876550"/>
+          <a:ext cx="1143000" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pet</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ToShelter</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01A0668E-467F-47A3-AA0F-88EBD06752A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="755650" y="2876550"/>
+          <a:ext cx="1143000" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Client</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>ToEmployee</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
       <xdr:row>9</xdr:row>
@@ -842,26 +1052,82 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33472579-6C8A-4CE4-8D0A-CCE226BE318D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F57F4097-2845-4B7C-A30E-E3D3AECEAD23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="21" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1327150" y="1704975"/>
+          <a:ext cx="0" cy="1171575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{637C4152-C19B-403C-8488-5EBFEE2AE87B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="0"/>
-          <a:endCxn id="2" idx="2"/>
+          <a:endCxn id="21" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1327150" y="1704975"/>
-          <a:ext cx="0" cy="1222375"/>
+          <a:off x="1327150" y="3562350"/>
+          <a:ext cx="0" cy="1066800"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -891,33 +1157,145 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E08C9FAA-B5FD-4D8D-B19E-72F19D7A863D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="18" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1898650" y="4972050"/>
+          <a:ext cx="1089025" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>473075</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{416DD05A-49AD-47B5-B609-D76FFB8181BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098F6DEC-89BA-4722-803A-903D1DBB6D3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="4" idx="1"/>
-          <a:endCxn id="5" idx="3"/>
+          <a:endCxn id="18" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1898650" y="3270250"/>
-          <a:ext cx="3295650" cy="0"/>
+          <a:off x="4130675" y="4972050"/>
+          <a:ext cx="1063625" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9998E6A-44F1-40A0-8CC1-8BBB47621411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="0"/>
+          <a:endCxn id="20" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5765800" y="3562350"/>
+          <a:ext cx="0" cy="1066800"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -954,26 +1332,26 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3445FD6D-F6F8-441A-B61D-5719C0380116}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7DCEBE4-643B-4E21-8BE3-67E48A94DFF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="0"/>
-          <a:endCxn id="3" idx="2"/>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="20" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
+        <a:xfrm>
           <a:off x="5765800" y="1704975"/>
-          <a:ext cx="0" cy="1222375"/>
+          <a:ext cx="0" cy="1171575"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1562,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D205A097-D829-4E1D-9A19-CC3B3BD7B270}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>